<commit_message>
Removed strain data not belonging to this study
</commit_message>
<xml_diff>
--- a/data/custom_data_import_files/DDB_PD_117_AMBR_custom.xlsx
+++ b/data/custom_data_import_files/DDB_PD_117_AMBR_custom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Documents\_phd\_data\custom_data_import_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\Desktop\Repeated-glucose-oscillations-at-high-cell-densities-influence-stress-related-functions-of-E.-coli\data\custom_data_import_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C32CA80-14EA-49AA-888D-846576E73590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6B5CFB-4EA8-483B-B58D-270D7D237873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="timepoint samples" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Timepoint Sample</t>
   </si>
@@ -135,96 +135,6 @@
   </si>
   <si>
     <t>DDB_PD_117_AMBR_R10__S05</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R11__S01</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R11__S02</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R11__S03</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R11__S04</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R11__S05</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R12__S01</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R12__S02</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R12__S03</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R12__S04</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R12__S05</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R13__S01</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R13__S02</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R13__S03</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R13__S04</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R13__S05</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R14__S01</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R14__S02</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R14__S03</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R14__S04</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R14__S05</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R15__S01</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R15__S02</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R15__S03</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R15__S04</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R15__S05</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R16__S01</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R16__S02</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R16__S03</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R16__S04</t>
-  </si>
-  <si>
-    <t>DDB_PD_117_AMBR_R16__S05</t>
   </si>
   <si>
     <t>Ammonium [g/L]</t>
@@ -323,9 +233,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -363,9 +273,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,26 +308,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -450,26 +343,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -643,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A61" sqref="A32:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +546,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1109,441 +985,6 @@
       </c>
       <c r="E31">
         <v>0.71102697443034901</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32">
-        <v>2.7999999999999137</v>
-      </c>
-      <c r="C32">
-        <v>2.8000000000001357</v>
-      </c>
-      <c r="D32">
-        <v>2.4999999999999467</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33">
-        <v>9.5000000000000639</v>
-      </c>
-      <c r="C33">
-        <v>9.5000000000000639</v>
-      </c>
-      <c r="D33">
-        <v>9.300000000000086</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34">
-        <v>22.000000000000352</v>
-      </c>
-      <c r="C34">
-        <v>21.249999999999879</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35">
-        <v>33.199999999999896</v>
-      </c>
-      <c r="C35">
-        <v>33.600000000000293</v>
-      </c>
-      <c r="D35">
-        <v>32.999999999999915</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36">
-        <v>52.499999999999993</v>
-      </c>
-      <c r="C36">
-        <v>52.500000000000213</v>
-      </c>
-      <c r="D36">
-        <v>52.699999999999967</v>
-      </c>
-      <c r="E36">
-        <v>1.83067356939535</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37">
-        <v>2.9000000000001247</v>
-      </c>
-      <c r="C37">
-        <v>2.8999999999999027</v>
-      </c>
-      <c r="D37">
-        <v>3.2999999999998586</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38">
-        <v>9.7000000000000419</v>
-      </c>
-      <c r="C38">
-        <v>10.000000000000009</v>
-      </c>
-      <c r="D38">
-        <v>9.9000000000000199</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39">
-        <v>18.750000000000153</v>
-      </c>
-      <c r="C39">
-        <v>20.999999999999908</v>
-      </c>
-      <c r="D39">
-        <v>19.750000000000043</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40">
-        <v>33.800000000000274</v>
-      </c>
-      <c r="C40">
-        <v>33.200000000000337</v>
-      </c>
-      <c r="D40">
-        <v>33.599999999999852</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41">
-        <v>52.4</v>
-      </c>
-      <c r="C41">
-        <v>52.200000000000024</v>
-      </c>
-      <c r="D41">
-        <v>52.300000000000011</v>
-      </c>
-      <c r="E41">
-        <v>1.74329274828533</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42">
-        <v>3.4000000000000696</v>
-      </c>
-      <c r="C42">
-        <v>3.2000000000000917</v>
-      </c>
-      <c r="D42">
-        <v>3.6000000000000476</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43">
-        <v>10.099999999999998</v>
-      </c>
-      <c r="C43">
-        <v>9.8000000000000309</v>
-      </c>
-      <c r="D43">
-        <v>9.3999999999998529</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44">
-        <v>21.249999999999879</v>
-      </c>
-      <c r="C44">
-        <v>21.499999999999851</v>
-      </c>
-      <c r="D44">
-        <v>22.250000000000323</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45">
-        <v>33.799999999999827</v>
-      </c>
-      <c r="C45">
-        <v>34.400000000000205</v>
-      </c>
-      <c r="D45">
-        <v>34.79999999999972</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46">
-        <v>54.00000000000005</v>
-      </c>
-      <c r="C46">
-        <v>53.700000000000081</v>
-      </c>
-      <c r="D46">
-        <v>54.300000000000011</v>
-      </c>
-      <c r="E46">
-        <v>1.8147546631977702</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47">
-        <v>4.0999999999999925</v>
-      </c>
-      <c r="C47">
-        <v>3.6000000000000476</v>
-      </c>
-      <c r="D47">
-        <v>3.4000000000000696</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48">
-        <v>10.099999999999998</v>
-      </c>
-      <c r="C48">
-        <v>9.3999999999998529</v>
-      </c>
-      <c r="D48">
-        <v>9.5999999999998309</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49">
-        <v>20.999999999999908</v>
-      </c>
-      <c r="C49">
-        <v>20.749999999999932</v>
-      </c>
-      <c r="D49">
-        <v>20.749999999999932</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50">
-        <v>31.80000000000005</v>
-      </c>
-      <c r="C50">
-        <v>32.000000000000028</v>
-      </c>
-      <c r="D50">
-        <v>32.79999999999994</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51">
-        <v>46.499999999999986</v>
-      </c>
-      <c r="C51">
-        <v>46.69999999999996</v>
-      </c>
-      <c r="D51">
-        <v>46.800000000000175</v>
-      </c>
-      <c r="E51">
-        <v>1.8909648217509101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>54</v>
-      </c>
-      <c r="B52">
-        <v>3.5999999999998256</v>
-      </c>
-      <c r="C52">
-        <v>3.7999999999998035</v>
-      </c>
-      <c r="D52">
-        <v>3.9000000000000146</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53">
-        <v>9.5999999999998309</v>
-      </c>
-      <c r="C53">
-        <v>9.3999999999998529</v>
-      </c>
-      <c r="D53">
-        <v>9.6000000000000529</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54">
-        <v>20.249999999999989</v>
-      </c>
-      <c r="C54">
-        <v>19.750000000000043</v>
-      </c>
-      <c r="D54">
-        <v>19.250000000000099</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55">
-        <v>32.000000000000028</v>
-      </c>
-      <c r="C55">
-        <v>32.000000000000028</v>
-      </c>
-      <c r="D55">
-        <v>32.79999999999994</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56">
-        <v>47.799999999999841</v>
-      </c>
-      <c r="C56">
-        <v>47.500000000000099</v>
-      </c>
-      <c r="D56">
-        <v>47.800000000000061</v>
-      </c>
-      <c r="E56">
-        <v>1.8033681654390299</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>59</v>
-      </c>
-      <c r="B57">
-        <v>3.4000000000000696</v>
-      </c>
-      <c r="C57">
-        <v>2.7999999999999137</v>
-      </c>
-      <c r="D57">
-        <v>3.2999999999998586</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58">
-        <v>10.099999999999998</v>
-      </c>
-      <c r="C58">
-        <v>9.7000000000000419</v>
-      </c>
-      <c r="D58">
-        <v>9.7000000000000419</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59">
-        <v>20.749999999999932</v>
-      </c>
-      <c r="C59">
-        <v>19.500000000000071</v>
-      </c>
-      <c r="D59">
-        <v>18.500000000000181</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>62</v>
-      </c>
-      <c r="B60">
-        <v>34.199999999999783</v>
-      </c>
-      <c r="C60">
-        <v>33.199999999999896</v>
-      </c>
-      <c r="D60">
-        <v>30.800000000000161</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>63</v>
-      </c>
-      <c r="B61">
-        <v>46.799999999999955</v>
-      </c>
-      <c r="C61">
-        <v>48.10000000000003</v>
-      </c>
-      <c r="D61">
-        <v>47.600000000000087</v>
-      </c>
-      <c r="E61">
-        <v>2.0386874350753099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>